<commit_message>
Fixed link to slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonbryer/Dropbox (Personal)/School/Teaching/DAV5300 2025 Fall/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89FAE8DF-55A1-8B4E-891D-934DBD40EE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3763C909-4495-674E-869A-2F75F3A0B6C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="4000" windowWidth="25340" windowHeight="14540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -189,7 +189,7 @@
     <t>NO CLASS</t>
   </si>
   <si>
-    <t>01-Intro_to_Course</t>
+    <t>01-Intro_to_Course.html</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>